<commit_message>
Adding labels and more stations to roving
</commit_message>
<xml_diff>
--- a/lake_monitoring_for_report_appendix.xlsx
+++ b/lake_monitoring_for_report_appendix.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">Waterbody</t>
   </si>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Paul Lake</t>
   </si>
   <si>
-    <t xml:space="preserve">Pend d'Oreille River</t>
+    <t xml:space="preserve">Pend dOreille River</t>
   </si>
   <si>
     <t xml:space="preserve">Peter-Hope</t>
@@ -290,9 +290,6 @@
     <t xml:space="preserve">Slocan River</t>
   </si>
   <si>
-    <t xml:space="preserve">St. Mary's Lake</t>
-  </si>
-  <si>
     <t xml:space="preserve">St. Marys Lake</t>
   </si>
   <si>
@@ -300,9 +297,6 @@
   </si>
   <si>
     <t xml:space="preserve">Summit Lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surveyor's Lake</t>
   </si>
   <si>
     <t xml:space="preserve">Surveyors Lake</t>
@@ -1642,10 +1636,10 @@
         <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -1656,10 +1650,10 @@
         <v>94</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -1673,7 +1667,7 @@
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -1687,7 +1681,7 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -1712,10 +1706,10 @@
         <v>98</v>
       </c>
       <c r="B74" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -1740,10 +1734,10 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -1754,10 +1748,10 @@
         <v>101</v>
       </c>
       <c r="B77" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -1768,10 +1762,10 @@
         <v>102</v>
       </c>
       <c r="B78" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -1782,10 +1776,10 @@
         <v>103</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -1796,10 +1790,10 @@
         <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C80" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -1810,10 +1804,10 @@
         <v>105</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -1824,10 +1818,10 @@
         <v>106</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -1841,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -1852,10 +1846,10 @@
         <v>108</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -1866,10 +1860,10 @@
         <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -1894,40 +1888,12 @@
         <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89" t="s">
-        <v>9</v>
-      </c>
-      <c r="C89" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>